<commit_message>
Now using participant-centric aggregations
</commit_message>
<xml_diff>
--- a/data/xlsx/Metrics_Eval_Participant_data_for_BBAI.xlsx
+++ b/data/xlsx/Metrics_Eval_Participant_data_for_BBAI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DaveBabbitt\Documents\GitHub\itm-analysis-reporting\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CCB98D7-2A06-45F4-8321-49C20CC5CB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310C688F-596B-4CAE-9870-DE2C91BAB7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7560" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -706,26 +706,36 @@
   <dimension ref="A1:AA23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="U22" sqref="U22"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.3984375" customWidth="1"/>
-    <col min="3" max="3" width="51.19921875" customWidth="1"/>
-    <col min="4" max="4" width="54.8984375" customWidth="1"/>
-    <col min="5" max="8" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.09765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.69921875" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="9.09765625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5" customWidth="1"/>
-    <col min="19" max="19" width="13" customWidth="1"/>
-    <col min="20" max="23" width="9"/>
-    <col min="24" max="24" width="22.3984375" customWidth="1"/>
-    <col min="25" max="27" width="9"/>
+    <col min="16" max="16" width="14.09765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.59765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="46.8" x14ac:dyDescent="0.3">
@@ -813,19 +823,19 @@
     </row>
     <row r="2" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F2" s="1">
         <v>2</v>
@@ -835,25 +845,25 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1">
-        <v>1.3333333333333333</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="J2" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K2" s="1">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="L2" s="1">
-        <v>0.43477495859441906</v>
+        <v>0.42121150072988622</v>
       </c>
       <c r="M2" s="1">
-        <v>0.34832616000671396</v>
+        <v>0.36716416858070705</v>
       </c>
       <c r="N2" s="1">
         <v>1</v>
       </c>
       <c r="O2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2" s="1">
         <v>0.41666666666666663</v>
@@ -871,42 +881,42 @@
         <v>1</v>
       </c>
       <c r="U2" s="1">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="V2" s="1">
         <v>1</v>
       </c>
       <c r="W2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X2" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="1">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="Z2" s="1">
         <v>1</v>
       </c>
       <c r="AA2" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" s="1">
         <v>2</v>
@@ -916,25 +926,25 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1">
-        <v>0.66666666666666663</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="J3" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="K3" s="1">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="L3" s="1">
-        <v>0.42121150072988622</v>
+        <v>0.43477495859441906</v>
       </c>
       <c r="M3" s="1">
-        <v>0.36716416858070705</v>
+        <v>0.34832616000671396</v>
       </c>
       <c r="N3" s="1">
         <v>1</v>
       </c>
       <c r="O3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="1">
         <v>0.41666666666666663</v>
@@ -952,45 +962,45 @@
         <v>1</v>
       </c>
       <c r="U3" s="1">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="V3" s="1">
         <v>1</v>
       </c>
       <c r="W3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X3" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Y3" s="1">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="Z3" s="1">
         <v>1</v>
       </c>
       <c r="AA3" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -1003,28 +1013,28 @@
         <v>1</v>
       </c>
       <c r="K4" s="1">
-        <v>3.125</v>
+        <v>2.5</v>
       </c>
       <c r="L4" s="1">
-        <v>0.28987177663017472</v>
+        <v>0.33194876059361211</v>
       </c>
       <c r="M4" s="1">
-        <v>0.36508179815267516</v>
+        <v>0.39427792264136374</v>
       </c>
       <c r="N4" s="1">
         <v>0</v>
       </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4" s="1">
-        <v>0.31666666666666665</v>
+        <v>0.51666666666666661</v>
       </c>
       <c r="Q4" s="1">
-        <v>0.39999999999999997</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="R4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4" s="1">
         <v>0</v>
@@ -1033,13 +1043,13 @@
         <v>1</v>
       </c>
       <c r="U4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V4" s="1">
         <v>1</v>
       </c>
       <c r="W4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X4" s="1">
         <v>1</v>
@@ -1051,27 +1061,27 @@
         <v>1</v>
       </c>
       <c r="AA4" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -1084,28 +1094,28 @@
         <v>1</v>
       </c>
       <c r="K5" s="1">
-        <v>2.5</v>
+        <v>3.125</v>
       </c>
       <c r="L5" s="1">
-        <v>0.33194876059361211</v>
+        <v>0.28987177663017472</v>
       </c>
       <c r="M5" s="1">
-        <v>0.39427792264136374</v>
+        <v>0.36508179815267516</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
       </c>
       <c r="O5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P5" s="1">
-        <v>0.51666666666666661</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="Q5" s="1">
-        <v>0.46666666666666667</v>
+        <v>0.39999999999999997</v>
       </c>
       <c r="R5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5" s="1">
         <v>0</v>
@@ -1114,13 +1124,13 @@
         <v>1</v>
       </c>
       <c r="U5" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="V5" s="1">
         <v>1</v>
       </c>
       <c r="W5" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X5" s="1">
         <v>1</v>
@@ -1132,24 +1142,24 @@
         <v>1</v>
       </c>
       <c r="AA5" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E6" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
@@ -1159,19 +1169,19 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1">
-        <v>-0.66666666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="J6" s="1">
         <v>0.75</v>
       </c>
       <c r="K6" s="1">
-        <v>2.625</v>
+        <v>2.25</v>
       </c>
       <c r="L6" s="1">
-        <v>0.38765428361861248</v>
+        <v>0.56912358507976291</v>
       </c>
       <c r="M6" s="1">
-        <v>0.40825802605503686</v>
+        <v>0.42389024607430104</v>
       </c>
       <c r="N6" s="1">
         <v>1</v>
@@ -1180,54 +1190,54 @@
         <v>1</v>
       </c>
       <c r="P6" s="1">
-        <v>0.46666666666666667</v>
+        <v>0.3666666666666667</v>
       </c>
       <c r="Q6" s="1">
-        <v>0.47499999999999998</v>
+        <v>0.17500000000000002</v>
       </c>
       <c r="R6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S6" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6" s="1">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1">
+        <v>3</v>
+      </c>
+      <c r="V6" s="1">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1">
+        <v>2</v>
+      </c>
+      <c r="X6" s="1">
         <v>0.5</v>
       </c>
-      <c r="U6" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="V6" s="1">
-        <v>1</v>
-      </c>
-      <c r="W6" s="1">
-        <v>3</v>
-      </c>
-      <c r="X6" s="1">
-        <v>1</v>
-      </c>
       <c r="Y6" s="1">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="Z6" s="1">
         <v>1</v>
       </c>
       <c r="AA6" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -1240,43 +1250,43 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1">
-        <v>1</v>
+        <v>-0.66666666666666663</v>
       </c>
       <c r="J7" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="K7" s="1">
-        <v>2.75</v>
+        <v>2.625</v>
       </c>
       <c r="L7" s="1">
-        <v>0.32164135176465752</v>
+        <v>0.38765428361861248</v>
       </c>
       <c r="M7" s="1">
-        <v>0.34104448656617548</v>
+        <v>0.40825802605503686</v>
       </c>
       <c r="N7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7" s="1">
-        <v>0.31666666666666665</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="Q7" s="1">
-        <v>0.41666666666666663</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="R7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T7" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="U7" s="1">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="V7" s="1">
         <v>1</v>
@@ -1288,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="Y7" s="1">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="Z7" s="1">
         <v>1</v>
@@ -1299,16 +1309,16 @@
     </row>
     <row r="8" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1321,31 +1331,31 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1">
-        <v>1.3333333333333333</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1">
         <v>1</v>
       </c>
       <c r="K8" s="1">
-        <v>2.125</v>
+        <v>2.75</v>
       </c>
       <c r="L8" s="1">
-        <v>0.3259200369935864</v>
+        <v>0.32164135176465752</v>
       </c>
       <c r="M8" s="1">
-        <v>0.36994817436087346</v>
+        <v>0.34104448656617548</v>
       </c>
       <c r="N8" s="1">
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8" s="1">
         <v>0.31666666666666665</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.46666666666666667</v>
+        <v>0.41666666666666663</v>
       </c>
       <c r="R8" s="1">
         <v>0</v>
@@ -1363,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="W8" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X8" s="1">
         <v>1</v>
@@ -1375,24 +1385,24 @@
         <v>1</v>
       </c>
       <c r="AA8" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1402,31 +1412,31 @@
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1">
-        <v>0.33333333333333331</v>
+        <v>1.3333333333333333</v>
       </c>
       <c r="J9" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="K9" s="1">
-        <v>2.25</v>
+        <v>2.125</v>
       </c>
       <c r="L9" s="1">
-        <v>0.56912358507976291</v>
+        <v>0.3259200369935864</v>
       </c>
       <c r="M9" s="1">
-        <v>0.42389024607430104</v>
+        <v>0.36994817436087346</v>
       </c>
       <c r="N9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="1">
         <v>1</v>
       </c>
       <c r="P9" s="1">
-        <v>0.3666666666666667</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="Q9" s="1">
-        <v>0.17500000000000002</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="R9" s="1">
         <v>0</v>
@@ -1444,19 +1454,19 @@
         <v>1</v>
       </c>
       <c r="W9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X9" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Z9" s="1">
         <v>1</v>
       </c>
       <c r="AA9" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
@@ -1791,120 +1801,98 @@
     </row>
     <row r="14" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="E14" s="1">
-        <v>6</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>-0.66666666666666663</v>
-      </c>
-      <c r="J14" s="1">
-        <v>1</v>
-      </c>
-      <c r="K14" s="1">
-        <v>2.125</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
       <c r="L14" s="1">
-        <v>0.27891172563759103</v>
+        <v>0.46544164292066997</v>
       </c>
       <c r="M14" s="1">
-        <v>0.36100949464986498</v>
+        <v>0.3452432254047384</v>
       </c>
       <c r="N14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="1">
         <v>0</v>
       </c>
       <c r="P14" s="1">
-        <v>0.46666666666666667</v>
+        <v>0.3666666666666667</v>
       </c>
       <c r="Q14" s="1">
-        <v>0.46666666666666667</v>
+        <v>0.8</v>
       </c>
       <c r="R14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S14" s="1">
-        <v>0</v>
-      </c>
-      <c r="T14" s="1">
-        <v>1</v>
-      </c>
-      <c r="U14" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="V14" s="1">
-        <v>1</v>
-      </c>
-      <c r="W14" s="1">
-        <v>3</v>
-      </c>
-      <c r="X14" s="1">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="1">
-        <v>3</v>
-      </c>
-      <c r="Z14" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="1">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
     </row>
     <row r="15" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+        <v>87</v>
+      </c>
+      <c r="E15" s="1">
+        <v>6</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
       <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
       <c r="I15" s="1">
-        <v>0</v>
+        <v>-0.66666666666666663</v>
       </c>
       <c r="J15" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K15" s="1">
-        <v>1.25</v>
+        <v>2.125</v>
       </c>
       <c r="L15" s="1">
-        <v>0.32015633492270523</v>
+        <v>0.27891172563759103</v>
       </c>
       <c r="M15" s="1">
-        <v>0.34482711228855889</v>
+        <v>0.36100949464986498</v>
       </c>
       <c r="N15" s="1">
         <v>0</v>
@@ -1913,10 +1901,10 @@
         <v>0</v>
       </c>
       <c r="P15" s="1">
-        <v>0.625</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="Q15" s="1">
-        <v>0.3666666666666667</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="R15" s="1">
         <v>1</v>
@@ -1928,68 +1916,72 @@
         <v>1</v>
       </c>
       <c r="U15" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="V15" s="1">
+        <v>1</v>
+      </c>
+      <c r="W15" s="1">
         <v>3</v>
       </c>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
       <c r="X15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y15" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="Z15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D16" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="1">
-        <v>6</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="1">
         <v>0</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K16" s="1">
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="L16" s="1">
-        <v>0.33462215459050082</v>
+        <v>0.32015633492270523</v>
       </c>
       <c r="M16" s="1">
-        <v>0.37211571152488965</v>
+        <v>0.34482711228855889</v>
       </c>
       <c r="N16" s="1">
         <v>0</v>
       </c>
       <c r="O16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="1">
-        <v>0.46666666666666667</v>
+        <v>0.625</v>
       </c>
       <c r="Q16" s="1">
-        <v>0.31666666666666665</v>
+        <v>0.3666666666666667</v>
       </c>
       <c r="R16" s="1">
         <v>1</v>
@@ -2001,78 +1993,58 @@
         <v>1</v>
       </c>
       <c r="U16" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="V16" s="1">
-        <v>1</v>
-      </c>
-      <c r="W16" s="1">
         <v>3</v>
       </c>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
       <c r="X16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="Z16" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="1">
-        <v>3</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
     </row>
     <row r="17" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="E17" s="1">
-        <v>6</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0</v>
-      </c>
-      <c r="I17" s="1">
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="J17" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="K17" s="1">
-        <v>2.5</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
       <c r="L17" s="1">
-        <v>0.3197499692969078</v>
+        <v>0.4301070971416191</v>
       </c>
       <c r="M17" s="1">
-        <v>0.38300469809366428</v>
+        <v>0.36289658202601699</v>
       </c>
       <c r="N17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P17" s="1">
-        <v>0.51666666666666661</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="Q17" s="1">
-        <v>0.5</v>
+        <v>0.56666666666666665</v>
       </c>
       <c r="R17" s="1">
         <v>1</v>
@@ -2080,46 +2052,30 @@
       <c r="S17" s="1">
         <v>1</v>
       </c>
-      <c r="T17" s="1">
-        <v>1</v>
-      </c>
-      <c r="U17" s="1">
-        <v>2.5</v>
-      </c>
-      <c r="V17" s="1">
-        <v>1</v>
-      </c>
-      <c r="W17" s="1">
-        <v>2</v>
-      </c>
-      <c r="X17" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="Y17" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="Z17" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="1">
-        <v>2</v>
-      </c>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
     </row>
     <row r="18" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E18" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -2129,31 +2085,31 @@
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1">
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="J18" s="1">
         <v>1</v>
       </c>
       <c r="K18" s="1">
-        <v>2.625</v>
+        <v>2.5</v>
       </c>
       <c r="L18" s="1">
-        <v>0.38093978629899966</v>
+        <v>0.33462215459050082</v>
       </c>
       <c r="M18" s="1">
-        <v>0.39512649633164787</v>
+        <v>0.37211571152488965</v>
       </c>
       <c r="N18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="1">
         <v>1</v>
       </c>
       <c r="P18" s="1">
-        <v>0.51666666666666661</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="Q18" s="1">
-        <v>0.46666666666666667</v>
+        <v>0.31666666666666665</v>
       </c>
       <c r="R18" s="1">
         <v>1</v>
@@ -2165,136 +2121,190 @@
         <v>1</v>
       </c>
       <c r="U18" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="V18" s="1">
         <v>1</v>
       </c>
       <c r="W18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X18" s="1">
         <v>1</v>
       </c>
       <c r="Y18" s="1">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="Z18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA18" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="K19" s="1">
+        <v>2.5</v>
+      </c>
       <c r="L19" s="1">
-        <v>0.46544164292066997</v>
+        <v>0.3197499692969078</v>
       </c>
       <c r="M19" s="1">
-        <v>0.3452432254047384</v>
+        <v>0.38300469809366428</v>
       </c>
       <c r="N19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" s="1">
-        <v>0.3666666666666667</v>
+        <v>0.51666666666666661</v>
       </c>
       <c r="Q19" s="1">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="R19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="1">
         <v>1</v>
       </c>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
-      <c r="AA19" s="1"/>
+      <c r="T19" s="1">
+        <v>1</v>
+      </c>
+      <c r="U19" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="V19" s="1">
+        <v>1</v>
+      </c>
+      <c r="W19" s="1">
+        <v>2</v>
+      </c>
+      <c r="X19" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="Y19" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="Z19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="20" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E20" s="1">
-        <v>3</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
       <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="I20" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J20" s="1">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1">
+        <v>2.625</v>
+      </c>
       <c r="L20" s="1">
-        <v>0.4301070971416191</v>
+        <v>0.38093978629899966</v>
       </c>
       <c r="M20" s="1">
-        <v>0.36289658202601699</v>
+        <v>0.39512649633164787</v>
       </c>
       <c r="N20" s="1">
         <v>1</v>
       </c>
       <c r="O20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P20" s="1">
+        <v>0.51666666666666661</v>
+      </c>
+      <c r="Q20" s="1">
         <v>0.46666666666666667</v>
       </c>
-      <c r="Q20" s="1">
-        <v>0.56666666666666665</v>
-      </c>
       <c r="R20" s="1">
         <v>1</v>
       </c>
       <c r="S20" s="1">
-        <v>1</v>
-      </c>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="T20" s="1">
+        <v>1</v>
+      </c>
+      <c r="U20" s="1">
+        <v>2</v>
+      </c>
+      <c r="V20" s="1">
+        <v>1</v>
+      </c>
+      <c r="W20" s="1">
+        <v>2</v>
+      </c>
+      <c r="X20" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="21" spans="1:27" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -2462,9 +2472,12 @@
       <c r="AA23" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA23">
+    <sortCondition ref="A2:A23"/>
+  </sortState>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <ignoredErrors>
-    <ignoredError sqref="E1:K18 F23:K23 L1:S20 L21:S23 A21:A23 A1:A20 F20:K20 F19:K19 F21:K21 F22:K22" numberStoredAsText="1"/>
+    <ignoredError sqref="E1:K1 L1:S1 A1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>